<commit_message>
Deploying to gh-pages from  @ f08dbf124e0b5867241aff2a47aeca1a357b6cfc 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/9.1.2.xlsx
+++ b/en/downloads/data-excel/9.1.2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Воздушный транспорт, тыс. тонн</t>
   </si>
@@ -523,7 +523,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -646,6 +646,9 @@
     </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -971,21 +974,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="1" max="3" width="35.85546875" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="33.75" customHeight="1">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="42.75" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>38</v>
       </c>
@@ -1002,7 +1001,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1">
+    <row r="2" spans="1:20" ht="15.75" thickBot="1">
       <c r="A2" s="22"/>
       <c r="B2" s="23"/>
       <c r="C2" s="22"/>
@@ -1013,7 +1012,7 @@
       <c r="H2" s="22"/>
       <c r="I2" s="22"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+    <row r="3" spans="1:20" ht="15.75" thickBot="1">
       <c r="A3" s="24" t="s">
         <v>20</v>
       </c>
@@ -1071,15 +1070,18 @@
       <c r="S3" s="26">
         <v>2022</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="38.25">
-      <c r="A4" s="21" t="s">
+      <c r="T3" s="26">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="41.25" customHeight="1">
+      <c r="A4" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="43" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="27">
@@ -1130,8 +1132,11 @@
       <c r="S4" s="33">
         <v>10444.200000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="T4" s="33">
+        <v>11350.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="28" t="s">
         <v>23</v>
       </c>
@@ -1189,8 +1194,11 @@
       <c r="S5" s="35">
         <v>21.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="T5" s="35">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="28" t="s">
         <v>26</v>
       </c>
@@ -1248,8 +1256,11 @@
       <c r="S6" s="35">
         <v>7361.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="T6" s="35">
+        <v>7996.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="28" t="s">
         <v>29</v>
       </c>
@@ -1307,8 +1318,11 @@
       <c r="S7" s="35">
         <v>143.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="T7" s="35">
+        <v>145.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="28" t="s">
         <v>32</v>
       </c>
@@ -1366,8 +1380,11 @@
       <c r="S8" s="35">
         <v>844.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="T8" s="35">
+        <v>1060.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="28" t="s">
         <v>34</v>
       </c>
@@ -1423,8 +1440,11 @@
         <v>1090</v>
       </c>
       <c r="S9" s="35"/>
-    </row>
-    <row r="10" spans="1:19" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="T9" s="35">
+        <v>2126.6999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="1" customFormat="1" ht="37.5" customHeight="1">
       <c r="A10" s="29" t="s">
         <v>43</v>
       </c>
@@ -1482,8 +1502,11 @@
       <c r="S10" s="36" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" s="1" customFormat="1">
+      <c r="T10" s="36">
+        <v>2985.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="1" customFormat="1">
       <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
@@ -1541,8 +1564,11 @@
       <c r="S11" s="38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" s="1" customFormat="1">
+      <c r="T11" s="38">
+        <v>1085.5999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="1" customFormat="1">
       <c r="A12" s="16" t="s">
         <v>19</v>
       </c>
@@ -1600,8 +1626,11 @@
       <c r="S12" s="38" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" s="1" customFormat="1">
+      <c r="T12" s="38">
+        <v>1403.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="1" customFormat="1">
       <c r="A13" s="16" t="s">
         <v>21</v>
       </c>
@@ -1659,8 +1688,11 @@
       <c r="S13" s="38">
         <v>273.39999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" s="1" customFormat="1">
+      <c r="T13" s="38">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="1" customFormat="1">
       <c r="A14" s="17" t="s">
         <v>8</v>
       </c>
@@ -1718,8 +1750,11 @@
       <c r="S14" s="40" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="T14" s="40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A15" s="18" t="s">
         <v>9</v>
       </c>
@@ -1777,8 +1812,11 @@
       <c r="S15" s="42">
         <v>17.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="T15" s="42">
+        <v>231.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="15" t="s">
         <v>3</v>
       </c>

</xml_diff>